<commit_message>
altium and prezentacja update
</commit_message>
<xml_diff>
--- a/lista-podzespolow-koszty.xlsx
+++ b/lista-podzespolow-koszty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tech\konkursy\WETI-2025_26-Szymon_Filipkowski\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB50B967-23F0-40B2-8A60-8B0F9F88DF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDB2274-3A86-4717-A10C-BA0A54DCB6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{2487162F-7312-4791-B288-7A04B70D1E4B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
@@ -95,25 +95,22 @@
     <t>https://botland.com.pl/akcesoria-do-raspberry-pi-pico/18854-zestaw-zlacz-meskich-do-gpio-raspberry-pi-pico-5904422328511.html</t>
   </si>
   <si>
-    <t>https://pl.rs-online.com/web/p/mikrokontrolery/2615535?gb=s</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>price from contest rules</t>
-  </si>
-  <si>
-    <t>price from contest rules - https://www.digikey.pl/pl/products/detail/texas-instruments/TLV2462CDGKR/1677686</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
     <t>100nf</t>
   </si>
   <si>
-    <t>STM32C011</t>
+    <t>STM32C031</t>
+  </si>
+  <si>
+    <t>https://pl.rs-online.com/web/p/mikrokontrolery/0214865?gb=s</t>
+  </si>
+  <si>
+    <t>https://www.digikey.pl/pl/products/detail/texas-instruments/TLV2462CDGKR/1677686</t>
   </si>
 </sst>
 </file>
@@ -562,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00AEF6D-22CF-4E98-8477-722CB40CBB7C}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -608,7 +605,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -620,16 +617,14 @@
         <f t="shared" ref="E2:E4" si="0">D2*C2</f>
         <v>0.15</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -641,9 +636,7 @@
         <f t="shared" ref="E3" si="1">D3*C3</f>
         <v>0.3</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -663,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -683,9 +676,7 @@
         <f>D5*C5</f>
         <v>0.6</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -704,7 +695,7 @@
         <f>D6*C6</f>
         <v>3.8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -713,19 +704,20 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" s="7">
-        <v>3.8</v>
+        <v>6.67</v>
       </c>
       <c r="E7" s="7">
-        <v>3.8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
+        <f>D7*C7</f>
+        <v>6.67</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -745,25 +737,25 @@
         <f>D8*C8</f>
         <v>15</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B11" s="6">
         <f>SUM(E2:E8)</f>
-        <v>24.65</v>
+        <v>27.52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="https://www.digikey.pl/pl/products/detail/texas-instruments/TLV2462CDGKR/1677686" xr:uid="{32FDC4A3-DFD1-4767-A910-8AA1D4C825D0}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{32FDC4A3-DFD1-4767-A910-8AA1D4C825D0}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{E7316A79-6C64-423F-83DD-473B4F65F14A}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{D2CBD7B4-3F2D-44EA-8440-6C76DEA374F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>